<commit_message>
Adding alternative descriptions to safety goals SG1 to SG3
</commit_message>
<xml_diff>
--- a/org.panorama-research.waters-2019.requirements/waters-challenge-2019-requirements_v2_proposal.xlsx
+++ b/org.panorama-research.waters-2019.requirements/waters-challenge-2019-requirements_v2_proposal.xlsx
@@ -37,6 +37,53 @@
     <author>Bjoern Koopmann</author>
   </authors>
   <commentList>
+    <comment ref="D15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bjoern Koopmann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Alternative: "The system shall prevent omitting breaking maneuvers to avoid collisions with obstacles."</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Alternative: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>"The system shall prevent omitting avoidance maneuvers to avoid collisions with obstacles, if safe."</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D130" authorId="0" shapeId="0">
       <text>
         <r>
@@ -212,9 +259,6 @@
     <t>The system shall be aware of its current position at all times.</t>
   </si>
   <si>
-    <t>The system shall avoid unintended acceleration.</t>
-  </si>
-  <si>
     <t>The system shall do a sanity check on the calculated speed profile to avoid unintended acceleration.</t>
   </si>
   <si>
@@ -654,6 +698,9 @@
   </si>
   <si>
     <t>The system shall reliably perform a breaking maneuver to avoid collisions with obstacles.</t>
+  </si>
+  <si>
+    <t>The system shall prevent unintended acceleration.</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1201,7 @@
   <dimension ref="A1:AL149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -1176,10 +1223,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>1</v>
@@ -1188,33 +1235,33 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>133</v>
-      </c>
       <c r="D2" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -1222,13 +1269,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -1239,10 +1286,10 @@
         <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -1250,13 +1297,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
@@ -1264,32 +1311,32 @@
         <v>7</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" s="35"/>
       <c r="C8" s="36"/>
@@ -1301,31 +1348,31 @@
         <v>29</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="27"/>
       <c r="D10" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="12"/>
       <c r="H10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1348,21 +1395,21 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="36"/>
@@ -1380,19 +1427,19 @@
     </row>
     <row r="15" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -1401,54 +1448,54 @@
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C17" s="33"/>
       <c r="D17" s="38"/>
     </row>
     <row r="18" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C19" s="33"/>
       <c r="D19" s="38"/>
     </row>
     <row r="20" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>11</v>
@@ -1456,21 +1503,21 @@
     </row>
     <row r="21" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C21" s="33"/>
       <c r="D21" s="38"/>
     </row>
     <row r="22" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>11</v>
@@ -1478,7 +1525,7 @@
     </row>
     <row r="23" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" s="33"/>
       <c r="D23" s="38"/>
@@ -1495,19 +1542,19 @@
     </row>
     <row r="26" spans="1:38" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -1516,18 +1563,18 @@
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="38"/>
@@ -1538,13 +1585,13 @@
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1554,10 +1601,10 @@
       <c r="B30" s="11"/>
       <c r="C30" s="28"/>
       <c r="D30" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="11"/>
@@ -1597,21 +1644,21 @@
     </row>
     <row r="31" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C31" s="33"/>
       <c r="D31" s="38"/>
     </row>
     <row r="32" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>11</v>
@@ -1619,21 +1666,21 @@
     </row>
     <row r="33" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C33" s="33"/>
       <c r="D33" s="38"/>
     </row>
     <row r="34" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H34" s="11" t="s">
         <v>11</v>
@@ -1641,21 +1688,21 @@
     </row>
     <row r="35" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C35" s="33"/>
       <c r="D35" s="38"/>
     </row>
     <row r="36" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H36" s="11" t="s">
         <v>11</v>
@@ -1663,7 +1710,7 @@
     </row>
     <row r="37" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
@@ -1672,15 +1719,15 @@
     </row>
     <row r="38" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="28"/>
       <c r="D38" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="11"/>
@@ -1720,7 +1767,7 @@
     </row>
     <row r="39" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
@@ -1773,19 +1820,19 @@
     </row>
     <row r="42" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G42" s="19">
         <v>3</v>
@@ -1798,19 +1845,19 @@
       <c r="B43" s="11"/>
       <c r="C43" s="28"/>
       <c r="D43" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B44" s="35"/>
       <c r="C44" s="36"/>
@@ -1824,19 +1871,19 @@
       <c r="B45" s="11"/>
       <c r="C45" s="28"/>
       <c r="D45" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B46" s="35"/>
       <c r="C46" s="36"/>
@@ -1850,19 +1897,19 @@
       <c r="B47" s="11"/>
       <c r="C47" s="28"/>
       <c r="D47" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B48" s="35"/>
       <c r="C48" s="36"/>
@@ -1876,19 +1923,19 @@
       <c r="B49" s="11"/>
       <c r="C49" s="28"/>
       <c r="D49" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B50" s="35"/>
       <c r="C50" s="36"/>
@@ -1902,10 +1949,10 @@
       <c r="B51" s="11"/>
       <c r="C51" s="28"/>
       <c r="D51" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="2" t="s">
@@ -1914,7 +1961,7 @@
     </row>
     <row r="52" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B52" s="35"/>
       <c r="C52" s="36"/>
@@ -1928,10 +1975,10 @@
       <c r="B53" s="11"/>
       <c r="C53" s="28"/>
       <c r="D53" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="2" t="s">
@@ -1940,30 +1987,30 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -1974,19 +2021,19 @@
     </row>
     <row r="58" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>48</v>
+        <v>195</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G58" s="19">
         <v>3</v>
@@ -1997,60 +2044,60 @@
         <v>16</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B63" s="35"/>
       <c r="C63" s="36"/>
@@ -2062,13 +2109,13 @@
         <v>17</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:38" x14ac:dyDescent="0.3">
@@ -2079,10 +2126,10 @@
         <v>32</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:38" x14ac:dyDescent="0.3">
@@ -2093,15 +2140,15 @@
         <v>33</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B67" s="35"/>
       <c r="C67" s="36"/>
@@ -2113,32 +2160,32 @@
         <v>18</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B70" s="35"/>
       <c r="C70" s="36"/>
@@ -2150,32 +2197,32 @@
         <v>19</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A72" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B73" s="35"/>
       <c r="C73" s="36"/>
@@ -2189,10 +2236,10 @@
       <c r="B74" s="11"/>
       <c r="C74" s="28"/>
       <c r="D74" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11" t="s">
@@ -2201,7 +2248,7 @@
     </row>
     <row r="75" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B75" s="35"/>
       <c r="C75" s="36"/>
@@ -2215,10 +2262,10 @@
       <c r="B76" s="11"/>
       <c r="C76" s="28"/>
       <c r="D76" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11" t="s">
@@ -2227,7 +2274,7 @@
     </row>
     <row r="77" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B77" s="35"/>
       <c r="C77" s="36"/>
@@ -2280,19 +2327,19 @@
     </row>
     <row r="80" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C80" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G80" s="19">
         <v>2</v>
@@ -2300,37 +2347,37 @@
     </row>
     <row r="81" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B81" s="11"/>
       <c r="C81" s="28"/>
       <c r="D81" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G81" s="11"/>
       <c r="H81" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="82" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B82" s="11"/>
       <c r="C82" s="28"/>
       <c r="D82" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="11"/>
       <c r="H82" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
@@ -2365,7 +2412,7 @@
     </row>
     <row r="83" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B83" s="35"/>
       <c r="C83" s="36"/>
@@ -2374,24 +2421,24 @@
     </row>
     <row r="84" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B84" s="11"/>
       <c r="C84" s="28"/>
       <c r="D84" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G84" s="11"/>
       <c r="H84" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="85" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B85" s="11"/>
       <c r="C85" s="28"/>
@@ -2399,12 +2446,12 @@
         <v>37</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="11"/>
       <c r="H85" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
@@ -2439,7 +2486,7 @@
     </row>
     <row r="86" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B86" s="11"/>
       <c r="C86" s="28"/>
@@ -2447,12 +2494,12 @@
         <v>33</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="11"/>
       <c r="H86" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
@@ -2487,7 +2534,7 @@
     </row>
     <row r="87" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B87" s="35"/>
       <c r="C87" s="36"/>
@@ -2496,29 +2543,29 @@
     </row>
     <row r="88" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A88" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B89" s="11"/>
       <c r="C89" s="28"/>
       <c r="D89" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="11"/>
@@ -2558,7 +2605,7 @@
     </row>
     <row r="90" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B90" s="35"/>
       <c r="C90" s="36"/>
@@ -2567,34 +2614,34 @@
     </row>
     <row r="91" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A91" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="28"/>
       <c r="D92" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="11"/>
       <c r="H92" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
@@ -2629,7 +2676,7 @@
     </row>
     <row r="93" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B93" s="35"/>
       <c r="C93" s="36"/>
@@ -2638,13 +2685,13 @@
     </row>
     <row r="94" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A94" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D94" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H94" s="11" t="s">
         <v>11</v>
@@ -2652,7 +2699,7 @@
     </row>
     <row r="95" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B95" s="35"/>
       <c r="C95" s="36"/>
@@ -2661,13 +2708,13 @@
     </row>
     <row r="96" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D96" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H96" s="11" t="s">
         <v>11</v>
@@ -2675,7 +2722,7 @@
     </row>
     <row r="97" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B97" s="35"/>
       <c r="C97" s="36"/>
@@ -2684,13 +2731,13 @@
     </row>
     <row r="98" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A98" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D98" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H98" s="11" t="s">
         <v>11</v>
@@ -2698,7 +2745,7 @@
     </row>
     <row r="99" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B99" s="35"/>
       <c r="C99" s="36"/>
@@ -2707,15 +2754,15 @@
     </row>
     <row r="100" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B100" s="11"/>
       <c r="C100" s="28"/>
       <c r="D100" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="11"/>
@@ -2755,7 +2802,7 @@
     </row>
     <row r="101" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B101" s="35"/>
       <c r="C101" s="36"/>
@@ -2764,15 +2811,15 @@
     </row>
     <row r="102" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B102" s="11"/>
       <c r="C102" s="28"/>
       <c r="D102" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="11"/>
@@ -2812,7 +2859,7 @@
     </row>
     <row r="103" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B103" s="35"/>
       <c r="C103" s="36"/>
@@ -2821,15 +2868,15 @@
     </row>
     <row r="104" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B104" s="11"/>
       <c r="C104" s="28"/>
       <c r="D104" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F104" s="2"/>
       <c r="G104" s="11"/>
@@ -2869,7 +2916,7 @@
     </row>
     <row r="105" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B105" s="35"/>
       <c r="C105" s="36"/>
@@ -2958,150 +3005,150 @@
     </row>
     <row r="108" spans="1:38" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C108" s="21"/>
       <c r="D108" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E108" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="109" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D109" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="110" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A110" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D110" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="111" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A111" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D111" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="112" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A112" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="113" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A113" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B113" s="25"/>
       <c r="C113" s="31"/>
       <c r="D113" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="114" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A114" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B114" s="25"/>
       <c r="C114" s="31"/>
       <c r="D114" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="115" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A115" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D115" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I115" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H115" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="116" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A116" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D116" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="117" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A117" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H117" s="2" t="s">
         <v>11</v>
@@ -3109,44 +3156,44 @@
     </row>
     <row r="118" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A118" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="119" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="120" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A120" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3231,126 +3278,126 @@
     </row>
     <row r="123" spans="1:38" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C123" s="21"/>
       <c r="D123" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E123" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="124" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A124" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="125" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B125" s="11"/>
       <c r="C125" s="13"/>
       <c r="D125" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G125" s="11"/>
       <c r="H125" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="126" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B126" s="11"/>
       <c r="C126" s="28"/>
       <c r="D126" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G126" s="11"/>
       <c r="H126" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="127" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A127" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D127" s="17" t="s">
         <v>30</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="128" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D128" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="129" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A129" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D129" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="130" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A130" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B130" s="24"/>
       <c r="C130" s="29"/>
       <c r="D130" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="131" spans="1:38" x14ac:dyDescent="0.3">
@@ -3367,19 +3414,19 @@
     </row>
     <row r="133" spans="1:38" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C133" s="21"/>
       <c r="D133" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E133" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="134" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B134" s="11"/>
       <c r="C134" s="28"/>
@@ -3387,12 +3434,12 @@
         <v>36</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F134" s="2"/>
       <c r="G134" s="11"/>
       <c r="H134" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I134" s="2"/>
       <c r="J134" s="2"/>
@@ -3427,23 +3474,23 @@
     </row>
     <row r="135" spans="1:38" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B135" s="11"/>
       <c r="C135" s="28"/>
       <c r="D135" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F135" s="2"/>
       <c r="G135" s="11"/>
       <c r="H135" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
@@ -3477,22 +3524,22 @@
     </row>
     <row r="136" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B136" s="11"/>
       <c r="C136" s="28"/>
       <c r="D136" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G136" s="11"/>
       <c r="H136" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I136" s="2"/>
       <c r="J136" s="2"/>
@@ -3527,22 +3574,22 @@
     </row>
     <row r="137" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B137" s="11"/>
       <c r="C137" s="28"/>
       <c r="D137" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G137" s="11"/>
       <c r="H137" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I137" s="2"/>
       <c r="J137" s="2"/>
@@ -3631,7 +3678,7 @@
         <v>35</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F143" s="2"/>
       <c r="G143" s="11"/>
@@ -3647,7 +3694,7 @@
         <v>35</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F144" s="2"/>
       <c r="G144" s="11"/>
@@ -3690,7 +3737,7 @@
         <v>35</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F145" s="2"/>
       <c r="G145" s="11"/>
@@ -3700,12 +3747,12 @@
     </row>
     <row r="148" spans="4:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D148" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="149" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D149" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>